<commit_message>
oppdatert med siste forbrukstall
</commit_message>
<xml_diff>
--- a/src/data/elforbruk/data.xlsx
+++ b/src/data/elforbruk/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magne.syljuasen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magne.syljuasen\kode\streamlit-kolbotn\src\data\elforbruk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA5617B-15F0-4EAE-8093-DF10446079A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A5CE17-45D1-4A30-A798-D10FDC23DFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{26C3DC0C-75B4-4581-8E27-C67A55B42F5C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>01.11.2023</t>
   </si>
@@ -189,13 +189,58 @@
   </si>
   <si>
     <t>kWh</t>
+  </si>
+  <si>
+    <t>20.12.2023</t>
+  </si>
+  <si>
+    <t>21.12.2023</t>
+  </si>
+  <si>
+    <t>22.12.2023</t>
+  </si>
+  <si>
+    <t>23.12.2023</t>
+  </si>
+  <si>
+    <t>24.12.2023</t>
+  </si>
+  <si>
+    <t>25.12.2023</t>
+  </si>
+  <si>
+    <t>26.12.2023</t>
+  </si>
+  <si>
+    <t>27.12.2023</t>
+  </si>
+  <si>
+    <t>28.12.2023</t>
+  </si>
+  <si>
+    <t>29.12.2023</t>
+  </si>
+  <si>
+    <t>30.12.2023</t>
+  </si>
+  <si>
+    <t>31.12.2023</t>
+  </si>
+  <si>
+    <t>01.01.2024</t>
+  </si>
+  <si>
+    <t>02.01.2024</t>
+  </si>
+  <si>
+    <t>03.01.2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +268,30 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -241,21 +310,45 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="7" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="13">
     <cellStyle name="BoldColumn" xfId="1" xr:uid="{57C6C2F3-818B-4DF9-980D-A3ED02B7FE92}"/>
+    <cellStyle name="BoldColumn 2" xfId="5" xr:uid="{81129D5D-4AA3-4F5C-82ED-3A2A8D45C533}"/>
     <cellStyle name="Decimal" xfId="2" xr:uid="{71AFB997-4F4C-440B-9D05-2623244C3E50}"/>
+    <cellStyle name="Decimal 2" xfId="7" xr:uid="{48F91543-F908-4990-9DAF-B8FEE439D91B}"/>
+    <cellStyle name="Default" xfId="4" xr:uid="{49C4D594-2FEE-4FDF-B11D-1D651AEE88B0}"/>
+    <cellStyle name="Integer" xfId="9" xr:uid="{518B2750-55B6-4DEB-8C6E-121FC18455BF}"/>
+    <cellStyle name="IntegerBold" xfId="8" xr:uid="{74640F3F-A532-4238-A065-C85C0A3C7362}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{60B16E02-AAA4-4BEE-ABF9-40446C3D3839}"/>
+    <cellStyle name="Number" xfId="12" xr:uid="{A193B16F-7BC5-4C36-8978-91DF8118C083}"/>
+    <cellStyle name="NumberBoldStyle" xfId="11" xr:uid="{CBE3E8E4-F6D3-4172-A433-12A29D9F0A8C}"/>
+    <cellStyle name="ShortLocalizedDate" xfId="10" xr:uid="{E4EA96FD-3CD6-4B1E-8E01-38AC04825CDD}"/>
+    <cellStyle name="StringLiteral" xfId="6" xr:uid="{7B6B50E5-39D1-43EC-9BDB-D3719D670151}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -567,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204B8C76-4F36-4290-B639-D5673E4BD54E}">
-  <dimension ref="A1:AH50"/>
+  <dimension ref="A1:AH65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -829,6 +922,19 @@
       <c r="B14" s="3">
         <v>88.7</v>
       </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
     </row>
     <row r="15" spans="1:34">
       <c r="A15" s="1" t="s">
@@ -837,6 +943,19 @@
       <c r="B15" s="3">
         <v>88</v>
       </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
     </row>
     <row r="16" spans="1:34">
       <c r="A16" s="1" t="s">
@@ -974,7 +1093,7 @@
         <v>1325.4</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -983,7 +1102,7 @@
       </c>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -992,7 +1111,7 @@
       </c>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -1001,7 +1120,7 @@
       </c>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -1010,7 +1129,7 @@
       </c>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -1019,7 +1138,7 @@
       </c>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -1028,7 +1147,7 @@
       </c>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -1037,7 +1156,7 @@
       </c>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -1046,7 +1165,7 @@
       </c>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -1055,7 +1174,7 @@
       </c>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -1066,7 +1185,7 @@
       <c r="D42" s="3"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -1074,7 +1193,7 @@
         <v>950.8</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -1082,7 +1201,7 @@
         <v>1109.4000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -1090,23 +1209,29 @@
         <v>1177.45</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="3">
         <v>1066.7</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B47" s="3">
         <v>749.9</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
@@ -1128,6 +1253,126 @@
       </c>
       <c r="B50" s="3">
         <v>801.05</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="5">
+        <v>904.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="5">
+        <v>1038.9000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="5">
+        <v>960.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="5">
+        <v>1296.8499999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="5">
+        <v>1334.1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="5">
+        <v>870.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="5">
+        <v>883.7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="5">
+        <v>984.85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" s="5">
+        <v>977.25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="5">
+        <v>868.9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" s="5">
+        <v>926.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" s="5">
+        <v>815.95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="7">
+        <v>780.8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="7">
+        <v>856.45</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" s="7">
+        <v>1393.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lagt til nye plot (Åsmund)
</commit_message>
<xml_diff>
--- a/src/data/elforbruk/data.xlsx
+++ b/src/data/elforbruk/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magne.syljuasen\kode\streamlit-kolbotn\src\data\elforbruk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asmund.fossum\Documents\streamlit-kolbotn\src\data\elforbruk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6F7396-8436-4A0A-AB4E-32A7912F6E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E996D8E-DD7A-4E1C-9515-F655CC047FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{26C3DC0C-75B4-4581-8E27-C67A55B42F5C}"/>
   </bookViews>
@@ -240,7 +240,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,6 +300,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -333,7 +339,7 @@
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="4" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -344,6 +350,7 @@
     <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="7" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="BoldColumn" xfId="1" xr:uid="{57C6C2F3-818B-4DF9-980D-A3ED02B7FE92}"/>
@@ -670,18 +677,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204B8C76-4F36-4290-B639-D5673E4BD54E}">
-  <dimension ref="A1:AH73"/>
+  <dimension ref="A1:AH94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="K57" sqref="K57"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -689,7 +696,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -697,7 +704,7 @@
         <v>81.599999999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -705,7 +712,7 @@
         <v>80.349999999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -745,7 +752,7 @@
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -785,7 +792,7 @@
       <c r="AG5" s="3"/>
       <c r="AH5" s="3"/>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -793,7 +800,7 @@
         <v>77.400000000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -833,7 +840,7 @@
       <c r="AG7" s="3"/>
       <c r="AH7" s="3"/>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -841,7 +848,7 @@
         <v>77.7</v>
       </c>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -849,7 +856,7 @@
         <v>77.75</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -860,7 +867,7 @@
       <c r="D10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -889,7 +896,7 @@
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -916,7 +923,7 @@
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
     </row>
-    <row r="13" spans="1:34">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -925,7 +932,7 @@
       </c>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:34">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -946,7 +953,7 @@
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
     </row>
-    <row r="15" spans="1:34">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -967,7 +974,7 @@
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
     </row>
-    <row r="16" spans="1:34">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -975,7 +982,7 @@
         <v>90.45</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -983,7 +990,7 @@
         <v>110.2</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -991,7 +998,7 @@
         <v>132.15</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -999,7 +1006,7 @@
         <v>253.3</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1007,7 +1014,7 @@
         <v>289.2</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1015,7 +1022,7 @@
         <v>167.05</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1023,7 +1030,7 @@
         <v>104.45</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1031,7 +1038,7 @@
         <v>86.8</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1039,7 +1046,7 @@
         <v>101.15</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1047,7 +1054,7 @@
         <v>126.25</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1055,7 +1062,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1063,7 +1070,7 @@
         <v>303.14999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1071,7 +1078,7 @@
         <v>721.5</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1079,7 +1086,7 @@
         <v>1352.22</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1087,7 +1094,7 @@
         <v>1066.28</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1095,7 +1102,7 @@
         <v>1117.3499999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -1103,7 +1110,7 @@
         <v>1325.4</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -1112,7 +1119,7 @@
       </c>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -1121,7 +1128,7 @@
       </c>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -1130,7 +1137,7 @@
       </c>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -1139,7 +1146,7 @@
       </c>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -1148,7 +1155,7 @@
       </c>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -1157,7 +1164,7 @@
       </c>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -1166,7 +1173,7 @@
       </c>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -1175,7 +1182,7 @@
       </c>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -1184,7 +1191,7 @@
       </c>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -1195,7 +1202,7 @@
       <c r="D42" s="3"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -1203,7 +1210,7 @@
         <v>950.8</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -1211,7 +1218,7 @@
         <v>1109.4000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -1219,7 +1226,7 @@
         <v>1177.45</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
@@ -1230,7 +1237,7 @@
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
@@ -1241,7 +1248,7 @@
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
@@ -1249,7 +1256,7 @@
         <v>710.6</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -1257,7 +1264,7 @@
         <v>824.55</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -1265,7 +1272,7 @@
         <v>801.05</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>51</v>
       </c>
@@ -1273,7 +1280,7 @@
         <v>904.2</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>52</v>
       </c>
@@ -1281,7 +1288,7 @@
         <v>1038.9000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>53</v>
       </c>
@@ -1289,7 +1296,7 @@
         <v>960.1</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>54</v>
       </c>
@@ -1297,7 +1304,7 @@
         <v>1296.8499999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>55</v>
       </c>
@@ -1305,7 +1312,7 @@
         <v>1334.1</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>56</v>
       </c>
@@ -1313,7 +1320,7 @@
         <v>870.8</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>57</v>
       </c>
@@ -1321,7 +1328,7 @@
         <v>883.7</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>58</v>
       </c>
@@ -1329,7 +1336,7 @@
         <v>984.85</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>59</v>
       </c>
@@ -1337,7 +1344,7 @@
         <v>977.25</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>60</v>
       </c>
@@ -1345,7 +1352,7 @@
         <v>868.9</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>61</v>
       </c>
@@ -1353,7 +1360,7 @@
         <v>926.2</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>62</v>
       </c>
@@ -1361,7 +1368,7 @@
         <v>815.95</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>63</v>
       </c>
@@ -1369,7 +1376,7 @@
         <v>780.8</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>64</v>
       </c>
@@ -1377,7 +1384,7 @@
         <v>856.45</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>65</v>
       </c>
@@ -1385,7 +1392,7 @@
         <v>1393.2</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <v>45295</v>
       </c>
@@ -1393,7 +1400,7 @@
         <v>1572.5</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
         <v>45296</v>
       </c>
@@ -1401,7 +1408,7 @@
         <v>1573.5</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
         <v>45297</v>
       </c>
@@ -1409,7 +1416,7 @@
         <v>1400.7</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="9">
         <v>45298</v>
       </c>
@@ -1417,7 +1424,7 @@
         <v>916.2</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="9">
         <v>45299</v>
       </c>
@@ -1425,7 +1432,7 @@
         <v>1574.3</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="9">
         <v>45300</v>
       </c>
@@ -1433,7 +1440,7 @@
         <v>1572.1</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
         <v>45301</v>
       </c>
@@ -1441,7 +1448,7 @@
         <v>1576.2</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
         <v>45302</v>
       </c>
@@ -1449,7 +1456,166 @@
         <v>1580.35</v>
       </c>
     </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="10">
+        <v>45303</v>
+      </c>
+      <c r="B74" s="3">
+        <v>1580.25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="10">
+        <v>45304</v>
+      </c>
+      <c r="B75" s="3">
+        <v>1428.05</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="9">
+        <v>45305</v>
+      </c>
+      <c r="B76" s="3">
+        <v>1333.95</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="9">
+        <v>45306</v>
+      </c>
+      <c r="B77" s="3">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="9">
+        <v>45307</v>
+      </c>
+      <c r="B78" s="3">
+        <v>1442.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="9">
+        <v>45308</v>
+      </c>
+      <c r="B79" s="3">
+        <v>1058.1500000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="9">
+        <v>45309</v>
+      </c>
+      <c r="B80" s="3">
+        <v>1194.4000000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="9">
+        <v>45310</v>
+      </c>
+      <c r="B81" s="3">
+        <v>1582.7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="9">
+        <v>45311</v>
+      </c>
+      <c r="B82" s="3">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="9">
+        <v>45312</v>
+      </c>
+      <c r="B83" s="3">
+        <v>1095.25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="10">
+        <v>45313</v>
+      </c>
+      <c r="B84" s="3">
+        <v>684.3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="10">
+        <v>45314</v>
+      </c>
+      <c r="B85" s="3">
+        <v>808.85</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="9">
+        <v>45315</v>
+      </c>
+      <c r="B86" s="3">
+        <v>685.25</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="9">
+        <v>45316</v>
+      </c>
+      <c r="B87" s="3">
+        <v>987.75</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="9">
+        <v>45317</v>
+      </c>
+      <c r="B88" s="3">
+        <v>959.45</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="9">
+        <v>45318</v>
+      </c>
+      <c r="B89" s="3">
+        <v>1078.4000000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="9">
+        <v>45319</v>
+      </c>
+      <c r="B90" s="3">
+        <v>566.29999999999995</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="9">
+        <v>45320</v>
+      </c>
+      <c r="B91" s="3">
+        <v>516.9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="9">
+        <v>45321</v>
+      </c>
+      <c r="B92" s="3">
+        <v>836.9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="9"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="10"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>